<commit_message>
Fixed formatting issue with the columns in the Excel spreadsheet for the QRDA Cat 1 checklist
</commit_message>
<xml_diff>
--- a/documents/cypress_ep_qrda_category_1_validation_checklist_04262013.xlsx
+++ b/documents/cypress_ep_qrda_category_1_validation_checklist_04262013.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="15975" yWindow="840" windowWidth="26115" windowHeight="18240" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="101" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="101" r:id="rId1"/>
     <sheet name="0002" sheetId="1" r:id="rId2"/>
     <sheet name="0004a" sheetId="2" r:id="rId3"/>
     <sheet name="0004b" sheetId="3" r:id="rId4"/>
@@ -2189,8 +2189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2268,6 +2268,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="47.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2470,6 +2475,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2699,6 +2710,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2917,6 +2933,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -3108,6 +3129,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -3500,6 +3526,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -3859,6 +3890,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4218,6 +4254,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4444,9 +4485,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4644,6 +4692,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4873,6 +4926,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5037,6 +5095,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5266,6 +5329,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5469,6 +5537,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5633,6 +5706,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -6203,6 +6281,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -6400,6 +6483,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -6673,6 +6762,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -6958,6 +7053,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -7101,6 +7202,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -7277,6 +7384,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -7479,6 +7592,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -7649,6 +7768,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -7732,6 +7856,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -7853,6 +7983,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="43.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -8042,6 +8177,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="60.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -8240,6 +8380,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -9203,6 +9348,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -9405,6 +9555,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -9575,6 +9730,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="46.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -9696,6 +9856,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="40.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -9828,6 +9993,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -9960,6 +10130,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -10070,6 +10244,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="41.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -10191,6 +10370,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -10312,6 +10497,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -10433,6 +10624,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -10576,6 +10773,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -10746,6 +10949,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -10933,6 +11142,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -11087,6 +11302,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -11263,6 +11484,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -11406,6 +11633,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -11631,6 +11863,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -11665,6 +11901,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -11890,6 +12131,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -12022,6 +12268,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -12143,6 +12394,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="72.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -12297,6 +12553,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -12499,6 +12760,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -12680,6 +12946,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -12823,6 +13094,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -12955,6 +13231,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -13148,6 +13429,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="55.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -13269,6 +13555,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="55.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -13941,6 +14232,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -14051,6 +14347,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="63.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -14194,6 +14495,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="52.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -14381,6 +14687,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="48.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -14568,6 +14879,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -14683,6 +14999,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="60.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -14894,6 +15215,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="69.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -15698,6 +16024,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -16348,6 +16679,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="41.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -16517,6 +16853,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="41.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -16978,6 +17319,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -17077,6 +17423,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -17176,6 +17527,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -17319,6 +17675,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -17451,6 +17812,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -17621,6 +17987,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -17731,6 +18102,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -17803,6 +18179,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -17913,6 +18294,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="53.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -18072,6 +18458,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="54.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -18171,6 +18562,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -18287,6 +18683,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="69.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -18905,6 +19306,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -19426,6 +19833,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -20184,9 +20597,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -20761,6 +21182,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -21335,6 +21762,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -21434,6 +21866,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -21533,6 +21971,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -21736,6 +22179,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="63.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -21928,6 +22376,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="67.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -22060,6 +22513,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="68.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -22192,6 +22650,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -22920,6 +23384,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -23516,6 +23986,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -24101,6 +24577,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -24222,6 +24703,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -24351,9 +24838,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -24875,6 +25368,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>